<commit_message>
Fixes an error with labeling where we were failing to account for the market share affected (20%); drops values from 0.1 to 0.02.
</commit_message>
<xml_diff>
--- a/InputData/bldgs/PPEIdtIL/Potential Perc Eff Improvement due to Impr Labeling.xlsx
+++ b/InputData/bldgs/PPEIdtIL/Potential Perc Eff Improvement due to Impr Labeling.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipI\InputData\bldgs\PPEIdtIL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rorvis\Dropbox (Energy InNovation)\My Documents\Energy Policy Solutions\US\Models\eps-us\InputData\bldgs\PPEIdtIL\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="24915" windowHeight="11055"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="24915" windowHeight="11055" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -487,8 +487,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD30"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -607,7 +607,9 @@
   </sheetPr>
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -636,14 +638,14 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>0.1</v>
+        <v>0.02</v>
       </c>
       <c r="C2">
         <f>B2</f>
-        <v>0.1</v>
+        <v>0.02</v>
       </c>
       <c r="D2">
-        <v>0.1</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -651,14 +653,14 @@
         <v>4</v>
       </c>
       <c r="B3">
-        <v>0.1</v>
+        <v>0.02</v>
       </c>
       <c r="C3">
         <f t="shared" ref="C3:C7" si="0">B3</f>
-        <v>0.1</v>
+        <v>0.02</v>
       </c>
       <c r="D3">
-        <v>0.1</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -696,14 +698,14 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>0.1</v>
+        <v>0.02</v>
       </c>
       <c r="C6">
         <f t="shared" si="0"/>
-        <v>0.1</v>
+        <v>0.02</v>
       </c>
       <c r="D6">
-        <v>0.1</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>